<commit_message>
modifier now writes to excell files
</commit_message>
<xml_diff>
--- a/datafiles/21-11 Demand Sheet Puyallup.xlsx
+++ b/datafiles/21-11 Demand Sheet Puyallup.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\STORPUYALLUP1-W10\The Stor-House Self Storage\Team Stor-House - Documents\Stores Files\Puyallup Files\Demand\"/>
     </mc:Choice>
@@ -1720,26 +1720,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="6" customWidth="1"/>
-    <col min="9" max="11" width="7.140625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" style="6" customWidth="1"/>
-    <col min="13" max="14" width="6.85546875" style="6" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="1"/>
-    <col min="19" max="19" width="8" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="1"/>
-    <col min="21" max="21" width="7.5703125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="7.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="6" width="10.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="6" width="5.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="6" width="6.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="6" width="6.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="6" width="6.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="6" width="6.42578125" collapsed="true"/>
+    <col min="9" max="11" customWidth="true" style="6" width="7.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="6" width="7.5703125" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" style="6" width="6.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="1" width="7.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" style="1" width="9.140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="20" max="20" style="1" width="9.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="23" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
@@ -5751,18 +5751,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="5.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" style="1" customWidth="1"/>
-    <col min="11" max="12" width="7.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="7.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="6.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="6.140625" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" style="1" width="5.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="7.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="7.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" style="1" width="7.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="14" max="14" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
@@ -7381,26 +7381,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" style="6" customWidth="1"/>
-    <col min="11" max="13" width="7.140625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" style="6" customWidth="1"/>
-    <col min="15" max="16" width="6.85546875" style="6" customWidth="1"/>
-    <col min="17" max="17" width="7.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="1"/>
-    <col min="19" max="19" width="8" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="1"/>
-    <col min="21" max="21" width="7.5703125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="7.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="6" width="5.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="6" width="6.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="6" width="7.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="6" width="6.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="6" width="5.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="6" width="6.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="6" width="5.7109375" collapsed="true"/>
+    <col min="11" max="13" customWidth="true" style="6" width="7.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="6" width="7.5703125" collapsed="true"/>
+    <col min="15" max="16" customWidth="true" style="6" width="6.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="18" max="18" style="1" width="9.140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="20" max="20" style="1" width="9.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="23" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.2">
@@ -8195,8 +8195,8 @@
       <c r="D18" s="16">
         <v>136</v>
       </c>
-      <c r="E18" s="91">
-        <v>111</v>
+      <c r="E18" s="91" t="n">
+        <v>113.0</v>
       </c>
       <c r="F18" s="31">
         <f t="shared" si="0"/>
@@ -8206,8 +8206,8 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="H18" s="91">
-        <v>7</v>
+      <c r="H18" s="91" t="n">
+        <v>9.0</v>
       </c>
       <c r="I18" s="74">
         <v>2</v>

</xml_diff>

<commit_message>
transfer rental method built and working
</commit_message>
<xml_diff>
--- a/datafiles/21-11 Demand Sheet Puyallup.xlsx
+++ b/datafiles/21-11 Demand Sheet Puyallup.xlsx
@@ -1915,11 +1915,11 @@
       </c>
       <c r="E6" s="22" t="n">
         <f>+'Input Tab'!E6</f>
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F6" s="31" t="n">
         <f t="shared" ref="F6:F29" si="0">E6/D6</f>
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G6" s="21" t="n">
         <f>'Input Tab'!H6</f>
@@ -2414,11 +2414,11 @@
       </c>
       <c r="E13" s="30" t="n">
         <f>+'Input Tab'!E18</f>
-        <v>114.0</v>
+        <v>115.0</v>
       </c>
       <c r="F13" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>0.8382352941176471</v>
+        <v>0.8455882352941176</v>
       </c>
       <c r="G13" s="30" t="n">
         <f>'Input Tab'!H18</f>
@@ -3801,15 +3801,15 @@
       </c>
       <c r="D33" s="16" t="n">
         <f>E6+E7</f>
-        <v>22.0</v>
+        <v>21.0</v>
       </c>
       <c r="E33" s="31" t="n">
         <f t="shared" ref="E33:E38" si="3">D33/C33</f>
-        <v>0.88</v>
+        <v>0.84</v>
       </c>
       <c r="F33" s="7" t="n">
         <f>C33-D33</f>
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G33" s="16" t="n">
         <f>G6+G7</f>
@@ -3852,7 +3852,7 @@
       </c>
       <c r="Q33" s="44" t="n">
         <f t="shared" ref="Q33:Q38" si="5">L33/F33</f>
-        <v>0.3333333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
@@ -3931,15 +3931,15 @@
       </c>
       <c r="D35" s="16" t="n">
         <f>E12+E13+E14+E15+E16</f>
-        <v>128.0</v>
+        <v>129.0</v>
       </c>
       <c r="E35" s="31" t="n">
         <f t="shared" si="3"/>
-        <v>0.8205128205128205</v>
+        <v>0.8269230769230769</v>
       </c>
       <c r="F35" s="7" t="n">
         <f>C35-D35</f>
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
       <c r="G35" s="16" t="n">
         <f>G12+G13+G14+G15+G16</f>
@@ -3982,7 +3982,7 @@
       </c>
       <c r="Q35" s="34" t="n">
         <f t="shared" si="5"/>
-        <v>0.6071428571428571</v>
+        <v>0.6296296296296297</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
@@ -7566,16 +7566,16 @@
       <c r="D6" s="14">
         <v>2</v>
       </c>
-      <c r="E6" s="71">
-        <v>2</v>
+      <c r="E6" s="71" t="n">
+        <v>1.0</v>
       </c>
       <c r="F6" s="26" t="n">
         <f t="shared" ref="F6:F34" si="0">E6/D6</f>
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G6" s="14" t="n">
         <f t="shared" ref="G6:G33" si="1">D6-E6</f>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H6" s="70"/>
       <c r="I6" s="71"/>
@@ -8202,15 +8202,15 @@
         <v>136</v>
       </c>
       <c r="E18" s="91" t="n">
-        <v>114.0</v>
+        <v>115.0</v>
       </c>
       <c r="F18" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>0.8382352941176471</v>
+        <v>0.8455882352941176</v>
       </c>
       <c r="G18" s="20" t="n">
         <f t="shared" si="1"/>
-        <v>22.0</v>
+        <v>21.0</v>
       </c>
       <c r="H18" s="91" t="n">
         <v>9.0</v>

</xml_diff>

<commit_message>
add demand method built and working
</commit_message>
<xml_diff>
--- a/datafiles/21-11 Demand Sheet Puyallup.xlsx
+++ b/datafiles/21-11 Demand Sheet Puyallup.xlsx
@@ -2265,7 +2265,7 @@
       <c r="I11" s="30"/>
       <c r="J11" s="30" t="n">
         <f>'Input Tab'!K12+'Input Tab'!K13+'Input Tab'!K14+'Input Tab'!K15+'Input Tab'!K16</f>
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="K11" s="30" t="n">
         <f>'Input Tab'!L12+'Input Tab'!L13+'Input Tab'!L14+'Input Tab'!L15+'Input Tab'!L16</f>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="M11" s="42" t="n">
         <f t="shared" si="1"/>
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="N11" s="23" t="n">
         <f>'Input Tab'!O12+'Input Tab'!O13+'Input Tab'!O14+'Input Tab'!O15+'Input Tab'!O16</f>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="Q11" s="34" t="n">
         <f t="shared" si="2"/>
-        <v>1.0</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -3658,7 +3658,7 @@
       <c r="I29" s="42"/>
       <c r="J29" s="42" t="n">
         <f>SUM(J6:J28)</f>
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="K29" s="50" t="n">
         <f>SUM(K6:K28)</f>
@@ -3670,7 +3670,7 @@
       </c>
       <c r="M29" s="42" t="n">
         <f>SUM(G29:L29)</f>
-        <v>58.0</v>
+        <v>59.0</v>
       </c>
       <c r="N29" s="42" t="n">
         <f>SUM(N6:N28)</f>
@@ -3686,7 +3686,7 @@
       </c>
       <c r="Q29" s="55" t="n">
         <f t="shared" si="2"/>
-        <v>0.7586206896551724</v>
+        <v>0.7457627118644068</v>
       </c>
     </row>
     <row r="30" spans="1:36" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3886,7 +3886,7 @@
       </c>
       <c r="I34" s="16" t="n">
         <f>+J8+J9+J10+J11</f>
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="J34" s="16" t="n">
         <f>K8+K9+K10+K11</f>
@@ -3898,7 +3898,7 @@
       </c>
       <c r="L34" s="15" t="n">
         <f>SUM(G34:K34)</f>
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="M34" s="16" t="n">
         <f>N8+N9+N10+N11</f>
@@ -3913,11 +3913,11 @@
       </c>
       <c r="P34" s="64" t="n">
         <f t="shared" si="4"/>
-        <v>0.9444444444444444</v>
+        <v>0.8947368421052632</v>
       </c>
       <c r="Q34" s="34" t="n">
         <f t="shared" si="5"/>
-        <v>0.8571428571428571</v>
+        <v>0.9047619047619048</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
@@ -4146,7 +4146,7 @@
       </c>
       <c r="I38" s="12" t="n">
         <f t="shared" si="7"/>
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="J38" s="12" t="n">
         <f t="shared" si="7"/>
@@ -4158,7 +4158,7 @@
       </c>
       <c r="L38" s="36" t="n">
         <f t="shared" si="7"/>
-        <v>58.0</v>
+        <v>59.0</v>
       </c>
       <c r="M38" s="12" t="n">
         <f t="shared" si="6"/>
@@ -4174,11 +4174,11 @@
       </c>
       <c r="P38" s="55" t="n">
         <f t="shared" si="4"/>
-        <v>0.7586206896551724</v>
+        <v>0.7457627118644068</v>
       </c>
       <c r="Q38" s="55" t="n">
         <f t="shared" si="5"/>
-        <v>0.6170212765957447</v>
+        <v>0.6276595744680851</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="9.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -4190,23 +4190,23 @@
       <c r="F39" s="7"/>
       <c r="G39" s="59" t="n">
         <f>G38/L38</f>
-        <v>0.3448275862068966</v>
+        <v>0.3389830508474576</v>
       </c>
       <c r="H39" s="59" t="n">
         <f>H38/L38</f>
-        <v>0.1724137931034483</v>
+        <v>0.1694915254237288</v>
       </c>
       <c r="I39" s="59" t="n">
         <f>I38/L38</f>
-        <v>0.29310344827586204</v>
+        <v>0.3050847457627119</v>
       </c>
       <c r="J39" s="59" t="n">
         <f>J38/L38</f>
-        <v>0.034482758620689655</v>
+        <v>0.03389830508474576</v>
       </c>
       <c r="K39" s="59" t="n">
         <f>K38/L38</f>
-        <v>0.15517241379310345</v>
+        <v>0.15254237288135594</v>
       </c>
       <c r="L39" s="67" t="n">
         <f>L38/L38</f>
@@ -8088,7 +8088,7 @@
       </c>
       <c r="J16" s="93"/>
       <c r="K16" s="93" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="L16" s="93">
         <v>1</v>
@@ -8098,7 +8098,7 @@
       </c>
       <c r="N16" s="42" t="n">
         <f t="shared" si="2"/>
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="O16" s="95" t="n">
         <v>12.0</v>
@@ -9150,7 +9150,7 @@
       </c>
       <c r="K34" s="47" t="n">
         <f t="shared" si="3"/>
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="L34" s="47" t="n">
         <f t="shared" si="3"/>
@@ -9162,7 +9162,7 @@
       </c>
       <c r="N34" s="47" t="n">
         <f t="shared" si="3"/>
-        <v>58.0</v>
+        <v>59.0</v>
       </c>
       <c r="O34" s="47" t="n">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
built basic button functionality
</commit_message>
<xml_diff>
--- a/datafiles/21-11 Demand Sheet Puyallup.xlsx
+++ b/datafiles/21-11 Demand Sheet Puyallup.xlsx
@@ -2265,7 +2265,7 @@
       <c r="I11" s="30"/>
       <c r="J11" s="30" t="n">
         <f>'Input Tab'!K12+'Input Tab'!K13+'Input Tab'!K14+'Input Tab'!K15+'Input Tab'!K16</f>
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="K11" s="30" t="n">
         <f>'Input Tab'!L12+'Input Tab'!L13+'Input Tab'!L14+'Input Tab'!L15+'Input Tab'!L16</f>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="M11" s="42" t="n">
         <f t="shared" si="1"/>
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="N11" s="23" t="n">
         <f>'Input Tab'!O12+'Input Tab'!O13+'Input Tab'!O14+'Input Tab'!O15+'Input Tab'!O16</f>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="Q11" s="34" t="n">
         <f t="shared" si="2"/>
-        <v>0.9230769230769231</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -3658,7 +3658,7 @@
       <c r="I29" s="42"/>
       <c r="J29" s="42" t="n">
         <f>SUM(J6:J28)</f>
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="K29" s="50" t="n">
         <f>SUM(K6:K28)</f>
@@ -3670,7 +3670,7 @@
       </c>
       <c r="M29" s="42" t="n">
         <f>SUM(G29:L29)</f>
-        <v>59.0</v>
+        <v>60.0</v>
       </c>
       <c r="N29" s="42" t="n">
         <f>SUM(N6:N28)</f>
@@ -3686,7 +3686,7 @@
       </c>
       <c r="Q29" s="55" t="n">
         <f t="shared" si="2"/>
-        <v>0.7457627118644068</v>
+        <v>0.7333333333333333</v>
       </c>
     </row>
     <row r="30" spans="1:36" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3886,7 +3886,7 @@
       </c>
       <c r="I34" s="16" t="n">
         <f>+J8+J9+J10+J11</f>
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="J34" s="16" t="n">
         <f>K8+K9+K10+K11</f>
@@ -3898,7 +3898,7 @@
       </c>
       <c r="L34" s="15" t="n">
         <f>SUM(G34:K34)</f>
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
       <c r="M34" s="16" t="n">
         <f>N8+N9+N10+N11</f>
@@ -3913,11 +3913,11 @@
       </c>
       <c r="P34" s="64" t="n">
         <f t="shared" si="4"/>
-        <v>0.8947368421052632</v>
+        <v>0.85</v>
       </c>
       <c r="Q34" s="34" t="n">
         <f t="shared" si="5"/>
-        <v>0.9047619047619048</v>
+        <v>0.9523809523809523</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
@@ -4146,7 +4146,7 @@
       </c>
       <c r="I38" s="12" t="n">
         <f t="shared" si="7"/>
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="J38" s="12" t="n">
         <f t="shared" si="7"/>
@@ -4158,7 +4158,7 @@
       </c>
       <c r="L38" s="36" t="n">
         <f t="shared" si="7"/>
-        <v>59.0</v>
+        <v>60.0</v>
       </c>
       <c r="M38" s="12" t="n">
         <f t="shared" si="6"/>
@@ -4174,11 +4174,11 @@
       </c>
       <c r="P38" s="55" t="n">
         <f t="shared" si="4"/>
-        <v>0.7457627118644068</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="Q38" s="55" t="n">
         <f t="shared" si="5"/>
-        <v>0.6276595744680851</v>
+        <v>0.6382978723404256</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="9.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -4190,23 +4190,23 @@
       <c r="F39" s="7"/>
       <c r="G39" s="59" t="n">
         <f>G38/L38</f>
-        <v>0.3389830508474576</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="H39" s="59" t="n">
         <f>H38/L38</f>
-        <v>0.1694915254237288</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I39" s="59" t="n">
         <f>I38/L38</f>
-        <v>0.3050847457627119</v>
+        <v>0.31666666666666665</v>
       </c>
       <c r="J39" s="59" t="n">
         <f>J38/L38</f>
-        <v>0.03389830508474576</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="K39" s="59" t="n">
         <f>K38/L38</f>
-        <v>0.15254237288135594</v>
+        <v>0.15</v>
       </c>
       <c r="L39" s="67" t="n">
         <f>L38/L38</f>
@@ -8088,7 +8088,7 @@
       </c>
       <c r="J16" s="93"/>
       <c r="K16" s="93" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="L16" s="93">
         <v>1</v>
@@ -8098,7 +8098,7 @@
       </c>
       <c r="N16" s="42" t="n">
         <f t="shared" si="2"/>
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="O16" s="95" t="n">
         <v>12.0</v>
@@ -9150,7 +9150,7 @@
       </c>
       <c r="K34" s="47" t="n">
         <f t="shared" si="3"/>
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="L34" s="47" t="n">
         <f t="shared" si="3"/>
@@ -9162,7 +9162,7 @@
       </c>
       <c r="N34" s="47" t="n">
         <f t="shared" si="3"/>
-        <v>59.0</v>
+        <v>60.0</v>
       </c>
       <c r="O34" s="47" t="n">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
tracker is fully working and null pointer issues have been resolved
</commit_message>
<xml_diff>
--- a/datafiles/21-11 Demand Sheet Puyallup.xlsx
+++ b/datafiles/21-11 Demand Sheet Puyallup.xlsx
@@ -1915,11 +1915,11 @@
       </c>
       <c r="E6" s="22" t="n">
         <f>+'Input Tab'!E6</f>
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F6" s="31" t="n">
         <f t="shared" ref="F6:F29" si="0">E6/D6</f>
-        <v>0.5</v>
+        <v>0.0</v>
       </c>
       <c r="G6" s="21" t="n">
         <f>'Input Tab'!H6</f>
@@ -1927,12 +1927,12 @@
       </c>
       <c r="H6" s="27" t="n">
         <f>'Input Tab'!I6</f>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="27" t="n">
         <f>'Input Tab'!K6</f>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K6" s="27" t="n">
         <f>'Input Tab'!L6</f>
@@ -1944,23 +1944,23 @@
       </c>
       <c r="M6" s="28" t="n">
         <f t="shared" ref="M6:M28" si="1">H6+I6+J6+K6+L6+G6</f>
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="N6" s="22" t="n">
         <f>'Input Tab'!O6</f>
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="O6" s="22" t="n">
         <f>'Input Tab'!P6</f>
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="P6" s="22" t="n">
         <f>'Input Tab'!Q6</f>
         <v>1.0</v>
       </c>
-      <c r="Q6" s="34" t="e">
+      <c r="Q6" s="34" t="n">
         <f t="shared" ref="Q6:Q29" si="2">N6/M6</f>
-        <v>#DIV/0!</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
@@ -1979,11 +1979,11 @@
       </c>
       <c r="E7" s="39" t="n">
         <f>+'Input Tab'!E7</f>
-        <v>20.0</v>
+        <v>19.0</v>
       </c>
       <c r="F7" s="40" t="n">
         <f t="shared" si="0"/>
-        <v>0.8695652173913043</v>
+        <v>0.8260869565217391</v>
       </c>
       <c r="G7" s="39" t="n">
         <f>'Input Tab'!H7</f>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="O7" s="39" t="n">
         <f>'Input Tab'!P7</f>
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="P7" s="38" t="n">
         <f>'Input Tab'!Q7</f>
@@ -2041,11 +2041,11 @@
       </c>
       <c r="E8" s="30" t="n">
         <f>'Input Tab'!E8+'Input Tab'!E9</f>
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="F8" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="G8" s="30" t="n">
         <f>'Input Tab'!H8+'Input Tab'!H9</f>
@@ -2103,11 +2103,11 @@
       </c>
       <c r="E9" s="30" t="n">
         <f>+'Input Tab'!E11</f>
-        <v>23.0</v>
+        <v>21.0</v>
       </c>
       <c r="F9" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>1.0</v>
+        <v>0.9130434782608695</v>
       </c>
       <c r="G9" s="30" t="n">
         <f>'Input Tab'!H11</f>
@@ -2120,7 +2120,7 @@
       <c r="I9" s="30"/>
       <c r="J9" s="30" t="n">
         <f>'Input Tab'!K11</f>
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K9" s="30" t="n">
         <f>'Input Tab'!L11</f>
@@ -2132,7 +2132,7 @@
       </c>
       <c r="M9" s="33" t="n">
         <f t="shared" si="1"/>
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="N9" s="23" t="n">
         <f>'Input Tab'!O11</f>
@@ -2148,7 +2148,7 @@
       </c>
       <c r="Q9" s="34" t="n">
         <f t="shared" si="2"/>
-        <v>0.6666666666666666</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="10" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -2167,15 +2167,15 @@
       </c>
       <c r="E10" s="30" t="n">
         <f>+'Input Tab'!E10</f>
-        <v>39.0</v>
+        <v>42.0</v>
       </c>
       <c r="F10" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>0.8125</v>
+        <v>0.875</v>
       </c>
       <c r="G10" s="30" t="n">
         <f>'Input Tab'!H10</f>
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H10" s="30" t="n">
         <f>'Input Tab'!I10</f>
@@ -2196,11 +2196,11 @@
       </c>
       <c r="M10" s="33" t="n">
         <f t="shared" si="1"/>
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="N10" s="23" t="n">
         <f>'Input Tab'!O10</f>
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="O10" s="30" t="n">
         <f>'Input Tab'!P10</f>
@@ -2248,11 +2248,11 @@
       </c>
       <c r="E11" s="30" t="n">
         <f>+'Input Tab'!E12+'Input Tab'!E13+'Input Tab'!E14+'Input Tab'!E15+'Input Tab'!E16</f>
-        <v>49.0</v>
+        <v>45.0</v>
       </c>
       <c r="F11" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>0.8166666666666667</v>
+        <v>0.75</v>
       </c>
       <c r="G11" s="30" t="n">
         <f>'Input Tab'!H12+'Input Tab'!H13+'Input Tab'!H14+'Input Tab'!H15+'Input Tab'!H16</f>
@@ -2265,7 +2265,7 @@
       <c r="I11" s="30"/>
       <c r="J11" s="30" t="n">
         <f>'Input Tab'!K12+'Input Tab'!K13+'Input Tab'!K14+'Input Tab'!K15+'Input Tab'!K16</f>
-        <v>7.0</v>
+        <v>0.0</v>
       </c>
       <c r="K11" s="30" t="n">
         <f>'Input Tab'!L12+'Input Tab'!L13+'Input Tab'!L14+'Input Tab'!L15+'Input Tab'!L16</f>
@@ -2277,15 +2277,15 @@
       </c>
       <c r="M11" s="42" t="n">
         <f t="shared" si="1"/>
-        <v>14.0</v>
+        <v>7.0</v>
       </c>
       <c r="N11" s="23" t="n">
         <f>'Input Tab'!O12+'Input Tab'!O13+'Input Tab'!O14+'Input Tab'!O15+'Input Tab'!O16</f>
-        <v>12.0</v>
+        <v>7.0</v>
       </c>
       <c r="O11" s="30" t="n">
         <f>'Input Tab'!P12+'Input Tab'!P13+'Input Tab'!P14+'Input Tab'!P15+'Input Tab'!P16</f>
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="P11" s="38" t="n">
         <f>'Input Tab'!Q12+'Input Tab'!Q13+'Input Tab'!Q14+'Input Tab'!Q15+'Input Tab'!Q16</f>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="Q11" s="34" t="n">
         <f t="shared" si="2"/>
-        <v>0.8571428571428571</v>
+        <v>1.0</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -2414,40 +2414,40 @@
       </c>
       <c r="E13" s="30" t="n">
         <f>+'Input Tab'!E18</f>
-        <v>115.0</v>
+        <v>129.0</v>
       </c>
       <c r="F13" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>0.8455882352941176</v>
+        <v>0.9485294117647058</v>
       </c>
       <c r="G13" s="30" t="n">
         <f>'Input Tab'!H18</f>
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="H13" s="30" t="n">
         <f>'Input Tab'!I18</f>
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="I13" s="30"/>
       <c r="J13" s="30" t="n">
         <f>'Input Tab'!K18</f>
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="K13" s="30" t="n">
         <f>'Input Tab'!L18</f>
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="L13" s="32" t="n">
         <f>+'Input Tab'!M18</f>
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="M13" s="33" t="n">
         <f t="shared" si="1"/>
-        <v>17.0</v>
+        <v>24.0</v>
       </c>
       <c r="N13" s="23" t="n">
         <f>'Input Tab'!O18</f>
-        <v>12.0</v>
+        <v>22.0</v>
       </c>
       <c r="O13" s="30" t="n">
         <f>'Input Tab'!P18</f>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="Q13" s="34" t="n">
         <f t="shared" si="2"/>
-        <v>0.7058823529411765</v>
+        <v>0.9166666666666666</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.2">
@@ -2478,11 +2478,11 @@
       </c>
       <c r="E14" s="30" t="n">
         <f>'Input Tab'!E19</f>
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F14" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G14" s="30" t="n">
         <f>'Input Tab'!H19</f>
@@ -2515,7 +2515,7 @@
       </c>
       <c r="O14" s="30" t="n">
         <f>'Input Tab'!P19</f>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P14" s="23" t="n">
         <f>'Input Tab'!Q19</f>
@@ -2770,11 +2770,11 @@
       </c>
       <c r="E18" s="30" t="n">
         <f>'Input Tab'!E23</f>
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="F18" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>0.6428571428571429</v>
+        <v>0.6785714285714286</v>
       </c>
       <c r="G18" s="30" t="n">
         <f>'Input Tab'!H23</f>
@@ -2787,7 +2787,7 @@
       <c r="I18" s="30"/>
       <c r="J18" s="30" t="n">
         <f>'Input Tab'!K23</f>
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="K18" s="30" t="n">
         <f>'Input Tab'!L23</f>
@@ -2799,11 +2799,11 @@
       </c>
       <c r="M18" s="33" t="n">
         <f t="shared" si="1"/>
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="N18" s="23" t="n">
         <f>'Input Tab'!O23</f>
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="O18" s="30" t="n">
         <f>'Input Tab'!P23</f>
@@ -3515,7 +3515,7 @@
       <c r="I27" s="30"/>
       <c r="J27" s="30" t="n">
         <f>'Input Tab'!K32</f>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K27" s="30" t="n">
         <f>'Input Tab'!L32</f>
@@ -3527,15 +3527,15 @@
       </c>
       <c r="M27" s="33" t="n">
         <f t="shared" si="1"/>
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="N27" s="23" t="n">
         <f>'Input Tab'!O32</f>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="O27" s="30" t="n">
         <f>'Input Tab'!P32</f>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P27" s="23" t="n">
         <f>'Input Tab'!Q32</f>
@@ -3543,7 +3543,7 @@
       </c>
       <c r="Q27" s="34" t="n">
         <f t="shared" si="2"/>
-        <v>0.0</v>
+        <v>0.2</v>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -3579,11 +3579,11 @@
       </c>
       <c r="E28" s="39" t="n">
         <f>'Input Tab'!E33</f>
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="F28" s="40" t="n">
         <f t="shared" si="0"/>
-        <v>1.0</v>
+        <v>0.875</v>
       </c>
       <c r="G28" s="39" t="n">
         <f>'Input Tab'!H33</f>
@@ -3616,7 +3616,7 @@
       </c>
       <c r="O28" s="39" t="n">
         <f>'Input Tab'!P33</f>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="P28" s="23" t="n">
         <f>'Input Tab'!Q33</f>
@@ -3641,52 +3641,52 @@
       </c>
       <c r="E29" s="50" t="n">
         <f>SUM(E6:E28)</f>
-        <v>448.0</v>
+        <v>455.0</v>
       </c>
       <c r="F29" s="54" t="n">
         <f t="shared" si="0"/>
-        <v>0.8265682656826568</v>
+        <v>0.8394833948339483</v>
       </c>
       <c r="G29" s="42" t="n">
         <f>SUM(G6:G28)</f>
-        <v>20.0</v>
+        <v>22.0</v>
       </c>
       <c r="H29" s="42" t="n">
         <f>SUM(H6:H28)</f>
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="I29" s="42"/>
       <c r="J29" s="42" t="n">
         <f>SUM(J6:J28)</f>
-        <v>19.0</v>
+        <v>18.0</v>
       </c>
       <c r="K29" s="50" t="n">
         <f>SUM(K6:K28)</f>
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="L29" s="42" t="n">
         <f>SUM(L6:L28)</f>
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="M29" s="42" t="n">
         <f>SUM(G29:L29)</f>
-        <v>60.0</v>
+        <v>66.0</v>
       </c>
       <c r="N29" s="42" t="n">
         <f>SUM(N6:N28)</f>
-        <v>44.0</v>
+        <v>56.0</v>
       </c>
       <c r="O29" s="50" t="n">
         <f>SUM(O6:O28)</f>
-        <v>32.0</v>
+        <v>37.0</v>
       </c>
       <c r="P29" s="191" t="n">
         <f>+N29-O3:O29</f>
-        <v>12.0</v>
+        <v>19.0</v>
       </c>
       <c r="Q29" s="55" t="n">
         <f t="shared" si="2"/>
-        <v>0.7333333333333333</v>
+        <v>0.8484848484848485</v>
       </c>
     </row>
     <row r="30" spans="1:36" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3801,15 +3801,15 @@
       </c>
       <c r="D33" s="16" t="n">
         <f>E6+E7</f>
-        <v>21.0</v>
+        <v>19.0</v>
       </c>
       <c r="E33" s="31" t="n">
         <f t="shared" ref="E33:E38" si="3">D33/C33</f>
-        <v>0.84</v>
+        <v>0.76</v>
       </c>
       <c r="F33" s="7" t="n">
         <f>C33-D33</f>
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="G33" s="16" t="n">
         <f>G6+G7</f>
@@ -3817,11 +3817,11 @@
       </c>
       <c r="H33" s="16" t="n">
         <f>H6+H7</f>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I33" s="16" t="n">
         <f>J6+J7</f>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J33" s="16" t="n">
         <f>K6+K7</f>
@@ -3833,26 +3833,26 @@
       </c>
       <c r="L33" s="15" t="n">
         <f>SUM(G33:K33)</f>
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="M33" s="16" t="n">
         <f>N6+N7</f>
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="N33" s="16" t="n">
         <f>O6+O7</f>
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="O33" s="16">
         <v>4</v>
       </c>
       <c r="P33" s="64" t="n">
         <f t="shared" ref="P33:P38" si="4">M33/L33</f>
-        <v>0.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="Q33" s="44" t="n">
         <f t="shared" ref="Q33:Q38" si="5">L33/F33</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
@@ -3866,19 +3866,19 @@
       </c>
       <c r="D34" s="16" t="n">
         <f>E8+E9+E10+E11</f>
-        <v>114.0</v>
+        <v>110.0</v>
       </c>
       <c r="E34" s="31" t="n">
         <f t="shared" si="3"/>
-        <v>0.8444444444444444</v>
+        <v>0.8148148148148148</v>
       </c>
       <c r="F34" s="7" t="n">
         <f>C34-D34</f>
-        <v>21.0</v>
+        <v>25.0</v>
       </c>
       <c r="G34" s="16" t="n">
         <f>G8+G9+G10+G11</f>
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H34" s="16" t="n">
         <f>H8+H9+H10+H11</f>
@@ -3886,7 +3886,7 @@
       </c>
       <c r="I34" s="16" t="n">
         <f>+J8+J9+J10+J11</f>
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="J34" s="16" t="n">
         <f>K8+K9+K10+K11</f>
@@ -3898,26 +3898,26 @@
       </c>
       <c r="L34" s="15" t="n">
         <f>SUM(G34:K34)</f>
-        <v>20.0</v>
+        <v>15.0</v>
       </c>
       <c r="M34" s="16" t="n">
         <f>N8+N9+N10+N11</f>
-        <v>17.0</v>
+        <v>15.0</v>
       </c>
       <c r="N34" s="16" t="n">
         <f>O8+O9+O10+O11</f>
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="O34" s="16">
         <v>13</v>
       </c>
       <c r="P34" s="64" t="n">
         <f t="shared" si="4"/>
-        <v>0.85</v>
+        <v>1.0</v>
       </c>
       <c r="Q34" s="34" t="n">
         <f t="shared" si="5"/>
-        <v>0.9523809523809523</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
@@ -3931,58 +3931,58 @@
       </c>
       <c r="D35" s="16" t="n">
         <f>E12+E13+E14+E15+E16</f>
-        <v>129.0</v>
+        <v>142.0</v>
       </c>
       <c r="E35" s="31" t="n">
         <f t="shared" si="3"/>
-        <v>0.8269230769230769</v>
+        <v>0.9102564102564102</v>
       </c>
       <c r="F35" s="7" t="n">
         <f>C35-D35</f>
-        <v>27.0</v>
+        <v>14.0</v>
       </c>
       <c r="G35" s="16" t="n">
         <f>G12+G13+G14+G15+G16</f>
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="H35" s="16" t="n">
         <f>H12+H13+H14+H15+H16</f>
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="I35" s="16" t="n">
         <f>+J12+J13+J14+J16+J15</f>
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="J35" s="16" t="n">
         <f>K12+K13+K14+K15+K16</f>
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="K35" s="16" t="n">
         <f>L12+L13+L14+L15+L16</f>
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="L35" s="15" t="n">
         <f>SUM(G35:K35)</f>
-        <v>17.0</v>
+        <v>24.0</v>
       </c>
       <c r="M35" s="16" t="n">
         <f>N12+N13+N14+N15+N16</f>
-        <v>12.0</v>
+        <v>22.0</v>
       </c>
       <c r="N35" s="16" t="n">
         <f>O12+O13+O14+O15+O16</f>
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="O35" s="16">
         <v>9</v>
       </c>
       <c r="P35" s="64" t="n">
         <f t="shared" si="4"/>
-        <v>0.7058823529411765</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="Q35" s="34" t="n">
         <f t="shared" si="5"/>
-        <v>0.6296296296296297</v>
+        <v>1.7142857142857142</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
@@ -3996,15 +3996,15 @@
       </c>
       <c r="D36" s="16" t="n">
         <f>E17+E18+E19+E20+E21+E22+E23</f>
-        <v>127.0</v>
+        <v>128.0</v>
       </c>
       <c r="E36" s="31" t="n">
         <f t="shared" si="3"/>
-        <v>0.7604790419161677</v>
+        <v>0.7664670658682635</v>
       </c>
       <c r="F36" s="7" t="n">
         <f>C36-D36</f>
-        <v>40.0</v>
+        <v>39.0</v>
       </c>
       <c r="G36" s="16" t="n">
         <f>+G17+G18+G19+G20+G21+G22+G23</f>
@@ -4016,7 +4016,7 @@
       </c>
       <c r="I36" s="116" t="n">
         <f>+J17+J18+J19+J20+J21+J22+J23</f>
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="J36" s="116" t="n">
         <f>+K17+K18+K19+K20+K21+K22+K23</f>
@@ -4028,11 +4028,11 @@
       </c>
       <c r="L36" s="15" t="n">
         <f>SUM(G36:K36)</f>
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="M36" s="16" t="n">
         <f>N17+N18+N19+N20+N21+N22+N23</f>
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="N36" s="16" t="n">
         <f>O17+O18+O19+O20+O21+O22+O23</f>
@@ -4043,11 +4043,11 @@
       </c>
       <c r="P36" s="64" t="n">
         <f t="shared" si="4"/>
-        <v>0.8461538461538461</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="Q36" s="34" t="n">
         <f t="shared" si="5"/>
-        <v>0.325</v>
+        <v>0.358974358974359</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
@@ -4061,15 +4061,15 @@
       </c>
       <c r="D37" s="43" t="n">
         <f>E24+E25+E26+E27+E28</f>
-        <v>57.0</v>
+        <v>56.0</v>
       </c>
       <c r="E37" s="31" t="n">
         <f t="shared" si="3"/>
-        <v>0.9661016949152542</v>
+        <v>0.9491525423728814</v>
       </c>
       <c r="F37" s="7" t="n">
         <f>C37-D37</f>
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="G37" s="43" t="n">
         <f>G24+G25+G26+G27+G28</f>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="I37" s="117" t="n">
         <f>J24+J25+J26+J27+J28</f>
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="J37" s="117" t="n">
         <f>K24+K25+K26+K27+K28</f>
@@ -4093,26 +4093,26 @@
       </c>
       <c r="L37" s="36" t="n">
         <f>SUM(G37:K37)</f>
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="M37" s="43" t="n">
         <f>N24+N25+N26+N27+N28</f>
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="N37" s="43" t="n">
         <f>O24+O25+O26+O27+O28</f>
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="O37" s="43">
         <v>6</v>
       </c>
       <c r="P37" s="64" t="n">
         <f t="shared" si="4"/>
-        <v>0.4444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="Q37" s="51" t="n">
         <f t="shared" si="5"/>
-        <v>4.5</v>
+        <v>3.3333333333333335</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
@@ -4126,47 +4126,47 @@
       </c>
       <c r="D38" s="12" t="n">
         <f>SUM(D33:D37)</f>
-        <v>448.0</v>
+        <v>455.0</v>
       </c>
       <c r="E38" s="49" t="n">
         <f t="shared" si="3"/>
-        <v>0.8265682656826568</v>
+        <v>0.8394833948339483</v>
       </c>
       <c r="F38" s="12" t="n">
         <f t="shared" ref="F38:O38" si="6">SUM(F33:F37)</f>
-        <v>94.0</v>
+        <v>87.0</v>
       </c>
       <c r="G38" s="65" t="n">
         <f t="shared" ref="G38:L38" si="7">SUM(G33:G37)</f>
-        <v>20.0</v>
+        <v>22.0</v>
       </c>
       <c r="H38" s="65" t="n">
         <f t="shared" si="7"/>
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="I38" s="12" t="n">
         <f t="shared" si="7"/>
-        <v>19.0</v>
+        <v>18.0</v>
       </c>
       <c r="J38" s="12" t="n">
         <f t="shared" si="7"/>
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="K38" s="37" t="n">
         <f t="shared" si="7"/>
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="L38" s="36" t="n">
         <f t="shared" si="7"/>
-        <v>60.0</v>
+        <v>66.0</v>
       </c>
       <c r="M38" s="12" t="n">
         <f t="shared" si="6"/>
-        <v>44.0</v>
+        <v>56.0</v>
       </c>
       <c r="N38" s="12" t="n">
         <f t="shared" si="6"/>
-        <v>32.0</v>
+        <v>37.0</v>
       </c>
       <c r="O38" s="12" t="n">
         <f t="shared" si="6"/>
@@ -4174,11 +4174,11 @@
       </c>
       <c r="P38" s="55" t="n">
         <f t="shared" si="4"/>
-        <v>0.7333333333333333</v>
+        <v>0.8484848484848485</v>
       </c>
       <c r="Q38" s="55" t="n">
         <f t="shared" si="5"/>
-        <v>0.6382978723404256</v>
+        <v>0.7586206896551724</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="9.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -4194,19 +4194,19 @@
       </c>
       <c r="H39" s="59" t="n">
         <f>H38/L38</f>
-        <v>0.16666666666666666</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="I39" s="59" t="n">
         <f>I38/L38</f>
-        <v>0.31666666666666665</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="J39" s="59" t="n">
         <f>J38/L38</f>
-        <v>0.03333333333333333</v>
+        <v>0.06060606060606061</v>
       </c>
       <c r="K39" s="59" t="n">
         <f>K38/L38</f>
-        <v>0.15</v>
+        <v>0.15151515151515152</v>
       </c>
       <c r="L39" s="67" t="n">
         <f>L38/L38</f>
@@ -7567,28 +7567,36 @@
         <v>2</v>
       </c>
       <c r="E6" s="71" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F6" s="26" t="n">
         <f t="shared" ref="F6:F34" si="0">E6/D6</f>
-        <v>0.5</v>
+        <v>0.0</v>
       </c>
       <c r="G6" s="14" t="n">
         <f t="shared" ref="G6:G33" si="1">D6-E6</f>
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H6" s="70"/>
-      <c r="I6" s="71"/>
+      <c r="I6" s="71" t="n">
+        <v>1.0</v>
+      </c>
       <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
+      <c r="K6" s="71" t="n">
+        <v>1.0</v>
+      </c>
       <c r="L6" s="71"/>
       <c r="M6" s="71"/>
       <c r="N6" s="28" t="n">
         <f t="shared" ref="N6:N33" si="2">SUM(H6:M6)</f>
-        <v>0.0</v>
-      </c>
-      <c r="O6" s="90"/>
-      <c r="P6" s="90"/>
+        <v>2.0</v>
+      </c>
+      <c r="O6" s="90" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P6" s="90" t="n">
+        <v>2.0</v>
+      </c>
       <c r="Q6" s="111">
         <v>1</v>
       </c>
@@ -7606,16 +7614,16 @@
       <c r="D7" s="38">
         <v>23</v>
       </c>
-      <c r="E7" s="93">
-        <v>20</v>
+      <c r="E7" s="93" t="n">
+        <v>19.0</v>
       </c>
       <c r="F7" s="40" t="n">
         <f t="shared" si="0"/>
-        <v>0.8695652173913043</v>
+        <v>0.8260869565217391</v>
       </c>
       <c r="G7" s="36" t="n">
         <f t="shared" si="1"/>
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H7" s="94"/>
       <c r="I7" s="93"/>
@@ -7630,8 +7638,8 @@
         <v>1.0</v>
       </c>
       <c r="O7" s="92"/>
-      <c r="P7" s="95">
-        <v>2</v>
+      <c r="P7" s="95" t="n">
+        <v>3.0</v>
       </c>
       <c r="Q7" s="113">
         <v>3</v>
@@ -7690,16 +7698,16 @@
       <c r="D9" s="15">
         <v>2</v>
       </c>
-      <c r="E9" s="74">
-        <v>2</v>
+      <c r="E9" s="74" t="n">
+        <v>1.0</v>
       </c>
       <c r="F9" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G9" s="15" t="n">
         <f t="shared" si="1"/>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H9" s="91"/>
       <c r="I9" s="74"/>
@@ -7728,18 +7736,20 @@
       <c r="D10" s="15">
         <v>48</v>
       </c>
-      <c r="E10" s="74">
-        <v>39</v>
+      <c r="E10" s="74" t="n">
+        <v>42.0</v>
       </c>
       <c r="F10" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>0.8125</v>
+        <v>0.875</v>
       </c>
       <c r="G10" s="15" t="n">
         <f t="shared" si="1"/>
-        <v>9.0</v>
-      </c>
-      <c r="H10" s="91"/>
+        <v>6.0</v>
+      </c>
+      <c r="H10" s="91" t="n">
+        <v>3.0</v>
+      </c>
       <c r="I10" s="74"/>
       <c r="J10" s="74"/>
       <c r="K10" s="74">
@@ -7751,10 +7761,10 @@
       </c>
       <c r="N10" s="33" t="n">
         <f t="shared" si="2"/>
-        <v>3.0</v>
-      </c>
-      <c r="O10" s="92">
-        <v>3</v>
+        <v>6.0</v>
+      </c>
+      <c r="O10" s="92" t="n">
+        <v>6.0</v>
       </c>
       <c r="P10" s="92">
         <v>2</v>
@@ -7776,30 +7786,28 @@
       <c r="D11" s="23">
         <v>23</v>
       </c>
-      <c r="E11" s="74">
-        <v>23</v>
+      <c r="E11" s="74" t="n">
+        <v>21.0</v>
       </c>
       <c r="F11" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>1.0</v>
+        <v>0.9130434782608695</v>
       </c>
       <c r="G11" s="15" t="n">
         <f t="shared" si="1"/>
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H11" s="91"/>
       <c r="I11" s="74"/>
       <c r="J11" s="74"/>
-      <c r="K11" s="74" t="n">
-        <v>1.0</v>
-      </c>
+      <c r="K11" s="74"/>
       <c r="L11" s="74"/>
       <c r="M11" s="74">
         <v>2</v>
       </c>
       <c r="N11" s="33" t="n">
         <f t="shared" si="2"/>
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="O11" s="92">
         <v>2</v>
@@ -7896,16 +7904,16 @@
       <c r="D13" s="15">
         <v>2</v>
       </c>
-      <c r="E13" s="74" t="n">
-        <v>0.0</v>
+      <c r="E13" s="74">
+        <v>1</v>
       </c>
       <c r="F13" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>0.0</v>
+        <v>0.5</v>
       </c>
       <c r="G13" s="15" t="n">
         <f t="shared" si="1"/>
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H13" s="91"/>
       <c r="I13" s="74"/>
@@ -7918,9 +7926,7 @@
         <v>0.0</v>
       </c>
       <c r="O13" s="92"/>
-      <c r="P13" s="92" t="n">
-        <v>1.0</v>
-      </c>
+      <c r="P13" s="92"/>
       <c r="Q13" s="112">
         <v>1</v>
       </c>
@@ -8069,16 +8075,16 @@
       <c r="D16" s="36">
         <v>48</v>
       </c>
-      <c r="E16" s="93" t="n">
-        <v>41.0</v>
+      <c r="E16" s="93">
+        <v>36</v>
       </c>
       <c r="F16" s="40" t="n">
         <f t="shared" si="0"/>
-        <v>0.8541666666666666</v>
+        <v>0.75</v>
       </c>
       <c r="G16" s="36" t="n">
         <f t="shared" si="1"/>
-        <v>7.0</v>
+        <v>12.0</v>
       </c>
       <c r="H16" s="94">
         <v>1</v>
@@ -8087,9 +8093,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="93"/>
-      <c r="K16" s="93" t="n">
-        <v>7.0</v>
-      </c>
+      <c r="K16" s="93"/>
       <c r="L16" s="93">
         <v>1</v>
       </c>
@@ -8098,10 +8102,10 @@
       </c>
       <c r="N16" s="42" t="n">
         <f t="shared" si="2"/>
-        <v>14.0</v>
-      </c>
-      <c r="O16" s="95" t="n">
-        <v>12.0</v>
+        <v>7.0</v>
+      </c>
+      <c r="O16" s="95">
+        <v>7</v>
       </c>
       <c r="P16" s="95">
         <v>3</v>
@@ -8202,38 +8206,38 @@
         <v>136</v>
       </c>
       <c r="E18" s="91" t="n">
-        <v>115.0</v>
+        <v>129.0</v>
       </c>
       <c r="F18" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>0.8455882352941176</v>
+        <v>0.9485294117647058</v>
       </c>
       <c r="G18" s="20" t="n">
         <f t="shared" si="1"/>
-        <v>21.0</v>
+        <v>7.0</v>
       </c>
       <c r="H18" s="91" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="I18" s="74">
-        <v>2</v>
+        <v>8.0</v>
+      </c>
+      <c r="I18" s="74" t="n">
+        <v>3.0</v>
       </c>
       <c r="J18" s="74"/>
       <c r="K18" s="74" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="L18" s="74">
-        <v>1</v>
-      </c>
-      <c r="M18" s="74">
-        <v>1</v>
+        <v>8.0</v>
+      </c>
+      <c r="L18" s="74" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="M18" s="74" t="n">
+        <v>2.0</v>
       </c>
       <c r="N18" s="33" t="n">
         <f t="shared" si="2"/>
-        <v>17.0</v>
-      </c>
-      <c r="O18" s="92">
-        <v>12</v>
+        <v>24.0</v>
+      </c>
+      <c r="O18" s="92" t="n">
+        <v>22.0</v>
       </c>
       <c r="P18" s="74">
         <v>5</v>
@@ -8255,16 +8259,16 @@
       <c r="D19" s="16">
         <v>2</v>
       </c>
-      <c r="E19" s="91">
-        <v>2</v>
+      <c r="E19" s="91" t="n">
+        <v>1.0</v>
       </c>
       <c r="F19" s="31" t="n">
         <f t="shared" si="0"/>
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G19" s="20" t="n">
         <f t="shared" si="1"/>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H19" s="91"/>
       <c r="I19" s="74"/>
@@ -8277,7 +8281,9 @@
         <v>0.0</v>
       </c>
       <c r="O19" s="92"/>
-      <c r="P19" s="74"/>
+      <c r="P19" s="74" t="n">
+        <v>1.0</v>
+      </c>
       <c r="Q19" s="112">
         <v>1</v>
       </c>
@@ -8442,33 +8448,33 @@
       <c r="D23" s="16">
         <v>28</v>
       </c>
-      <c r="E23" s="92">
-        <v>18</v>
+      <c r="E23" s="92" t="n">
+        <v>19.0</v>
       </c>
       <c r="F23" s="103" t="n">
         <f t="shared" si="0"/>
-        <v>0.6428571428571429</v>
+        <v>0.6785714285714286</v>
       </c>
       <c r="G23" s="20" t="n">
         <f t="shared" si="1"/>
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="H23" s="91"/>
       <c r="I23" s="74">
         <v>1</v>
       </c>
       <c r="J23" s="74"/>
-      <c r="K23" s="74">
-        <v>1</v>
+      <c r="K23" s="74" t="n">
+        <v>2.0</v>
       </c>
       <c r="L23" s="74"/>
       <c r="M23" s="74"/>
       <c r="N23" s="33" t="n">
         <f t="shared" si="2"/>
-        <v>2.0</v>
-      </c>
-      <c r="O23" s="92">
-        <v>2</v>
+        <v>3.0</v>
+      </c>
+      <c r="O23" s="92" t="n">
+        <v>3.0</v>
       </c>
       <c r="P23" s="74">
         <v>5</v>
@@ -9009,8 +9015,8 @@
       <c r="D32" s="16">
         <v>17</v>
       </c>
-      <c r="E32" s="92">
-        <v>17</v>
+      <c r="E32" s="92" t="n">
+        <v>17.0</v>
       </c>
       <c r="F32" s="103" t="n">
         <f t="shared" si="0"/>
@@ -9025,15 +9031,21 @@
       </c>
       <c r="I32" s="74"/>
       <c r="J32" s="74"/>
-      <c r="K32" s="74"/>
+      <c r="K32" s="74" t="n">
+        <v>1.0</v>
+      </c>
       <c r="L32" s="74"/>
       <c r="M32" s="74"/>
       <c r="N32" s="33" t="n">
         <f t="shared" si="2"/>
-        <v>4.0</v>
-      </c>
-      <c r="O32" s="92"/>
-      <c r="P32" s="74"/>
+        <v>5.0</v>
+      </c>
+      <c r="O32" s="92" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P32" s="74" t="n">
+        <v>1.0</v>
+      </c>
       <c r="Q32" s="112">
         <v>1</v>
       </c>
@@ -9067,16 +9079,16 @@
       <c r="D33" s="16">
         <v>8</v>
       </c>
-      <c r="E33" s="92">
-        <v>8</v>
+      <c r="E33" s="92" t="n">
+        <v>7.0</v>
       </c>
       <c r="F33" s="103" t="n">
         <f t="shared" si="0"/>
-        <v>1.0</v>
+        <v>0.875</v>
       </c>
       <c r="G33" s="20" t="n">
         <f t="shared" si="1"/>
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H33" s="91"/>
       <c r="I33" s="74"/>
@@ -9089,7 +9101,9 @@
         <v>0.0</v>
       </c>
       <c r="O33" s="92"/>
-      <c r="P33" s="74"/>
+      <c r="P33" s="74" t="n">
+        <v>1.0</v>
+      </c>
       <c r="Q33" s="112">
         <v>1</v>
       </c>
@@ -9126,23 +9140,23 @@
       </c>
       <c r="E34" s="47" t="n">
         <f>SUM(E6:E33)</f>
-        <v>448.0</v>
+        <v>455.0</v>
       </c>
       <c r="F34" s="69" t="n">
         <f t="shared" si="0"/>
-        <v>0.8265682656826568</v>
+        <v>0.8394833948339483</v>
       </c>
       <c r="G34" s="47" t="n">
         <f t="shared" ref="G34:Q34" si="3">SUM(G6:G33)</f>
-        <v>94.0</v>
+        <v>87.0</v>
       </c>
       <c r="H34" s="47" t="n">
         <f t="shared" si="3"/>
-        <v>20.0</v>
+        <v>22.0</v>
       </c>
       <c r="I34" s="47" t="n">
         <f t="shared" si="3"/>
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="J34" s="47" t="n">
         <f t="shared" si="3"/>
@@ -9150,27 +9164,27 @@
       </c>
       <c r="K34" s="47" t="n">
         <f t="shared" si="3"/>
-        <v>19.0</v>
+        <v>18.0</v>
       </c>
       <c r="L34" s="47" t="n">
         <f t="shared" si="3"/>
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="M34" s="47" t="n">
         <f t="shared" si="3"/>
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="N34" s="47" t="n">
         <f t="shared" si="3"/>
-        <v>60.0</v>
+        <v>66.0</v>
       </c>
       <c r="O34" s="47" t="n">
         <f t="shared" si="3"/>
-        <v>44.0</v>
+        <v>56.0</v>
       </c>
       <c r="P34" s="47" t="n">
         <f t="shared" si="3"/>
-        <v>32.0</v>
+        <v>37.0</v>
       </c>
       <c r="Q34" s="47" t="n">
         <f t="shared" si="3"/>

</xml_diff>